<commit_message>
L'endpoint /statistique fonctionne bien. Les 2 derniers indicateurs (méthode calculerStatistiqueAllEmployees())retournent le bon résultat
</commit_message>
<xml_diff>
--- a/Avancement TP SOAP REST.xlsx
+++ b/Avancement TP SOAP REST.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
   <si>
     <t>GET</t>
   </si>
@@ -78,6 +78,36 @@
   </si>
   <si>
     <t>EquipeServiceImpl: refactorisation de la récupération de l'instance de demoSoapJava7 par interface fonctionnelle</t>
+  </si>
+  <si>
+    <t>/statistique/</t>
+  </si>
+  <si>
+    <t>le chiffre affaire total</t>
+  </si>
+  <si>
+    <t>le benefice total (affaire - salaire)</t>
+  </si>
+  <si>
+    <t>le chiffre affaire max (nom de l 'employee + montant)</t>
+  </si>
+  <si>
+    <t>le chiffre affaire  min  (nom de l 'employee + montant)</t>
+  </si>
+  <si>
+    <t>employee le plus rentable</t>
+  </si>
+  <si>
+    <t>employee les moins rentable (liste &lt;nom de l 'employee + montant&gt; des employe dont le benefice &lt; benefice moyen )</t>
+  </si>
+  <si>
+    <t>OK, à verifier quantité</t>
+  </si>
+  <si>
+    <t>OK, je retourne un obj Employee, entier!</t>
+  </si>
+  <si>
+    <t>KO</t>
   </si>
 </sst>
 </file>
@@ -93,12 +123,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -113,8 +149,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,17 +432,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" customWidth="1"/>
     <col min="2" max="2" width="23.140625" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="3" max="3" width="108.140625" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" customWidth="1"/>
     <col min="6" max="6" width="24.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -507,6 +544,77 @@
         <v>17</v>
       </c>
     </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>